<commit_message>
added simple linear regression worksheet
</commit_message>
<xml_diff>
--- a/Statistics/Confidence_Intervals.xlsx
+++ b/Statistics/Confidence_Intervals.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A00742989\ShareFile\Personal Folders\Excel_Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Desktop\Excel_fun\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4672934-375A-413C-ACC4-B5FA6938E6E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" tabRatio="763" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="763" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Mean Sigma Unknown" sheetId="4" r:id="rId1"/>
@@ -24,12 +25,23 @@
     <definedName name="solver_ver" localSheetId="0" hidden="1">17</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">17</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Error</t>
   </si>
@@ -120,9 +132,6 @@
   </si>
   <si>
     <t>(Round up)</t>
-  </si>
-  <si>
-    <t>Choosing your theSample Size</t>
   </si>
   <si>
     <t xml:space="preserve">confidence </t>
@@ -219,7 +228,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -598,7 +607,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -713,7 +721,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>800</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -782,7 +790,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-1477.4246382850592</c:v>
+                  <c:v>172.15185516007287</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -849,7 +857,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3077.4246382850592</c:v>
+                  <c:v>227.84814483992713</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1066,7 +1074,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1506,7 +1513,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3607,7 +3613,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3683,7 +3695,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3718,7 +3736,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3753,7 +3777,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3832,7 +3862,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4136,41 +4172,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="1" max="1" width="4.1328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="1"/>
     <col min="4" max="4" width="5.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="5" width="23.1328125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="45"/>
     </row>
-    <row r="3" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="46"/>
       <c r="C3" s="47"/>
       <c r="E3" s="32" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F3" s="33"/>
       <c r="G3" s="34"/>
     </row>
-    <row r="4" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
@@ -4184,45 +4220,45 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="4">
-        <v>800</v>
+        <v>200</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4">
         <v>3536</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4">
-        <v>5393.38</v>
+        <v>56</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="20">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="E9" s="7" t="s">
@@ -4234,29 +4270,29 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B10" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="18">
         <f>1-C5</f>
         <v>0.95</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="23">
         <f>1-F5</f>
         <v>0.95</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B11" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="13">
         <f>_xlfn.T.INV(1-C5/2,C8-1)</f>
-        <v>2.0686576104190477</v>
+        <v>2.109815577833317</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>9</v>
@@ -4267,13 +4303,13 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B12" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="5">
         <f>_xlfn.CONFIDENCE.T(C5,C7,C8)</f>
-        <v>2277.4246382850606</v>
+        <v>27.848144839927116</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>14</v>
@@ -4283,22 +4319,22 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B13" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5">
         <f>C11*C7/SQRT(C8)</f>
-        <v>2277.4246382850592</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+        <v>27.848144839927119</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B14" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="5">
         <f>C6-C13</f>
-        <v>-1477.4246382850592</v>
+        <v>172.15185516007287</v>
       </c>
       <c r="E14" s="35" t="str">
         <f>CONCATENATE("To get a confidence level of ",TEXT(F10, "0%"), " with an error of no more than ", F7, " sample size should be ", F12, "." )</f>
@@ -4307,39 +4343,39 @@
       <c r="F14" s="36"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B15" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="14">
         <f>C6+C13</f>
-        <v>3077.4246382850592</v>
+        <v>227.84814483992713</v>
       </c>
       <c r="E15" s="38"/>
       <c r="F15" s="39"/>
       <c r="G15" s="40"/>
     </row>
-    <row r="16" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D16" s="22"/>
       <c r="E16" s="38"/>
       <c r="F16" s="39"/>
       <c r="G16" s="40"/>
     </row>
-    <row r="17" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="35" t="str">
         <f>"The mean is between "&amp;TEXT(C14,"0.00")&amp;" and "&amp;TEXT(C15,"0.00")&amp; " with "&amp;TEXT(C10, "0%")&amp; " confidence."</f>
-        <v>The mean is between -1477.42 and 3077.42 with 95% confidence.</v>
+        <v>The mean is between 172.15 and 227.85 with 95% confidence.</v>
       </c>
       <c r="C17" s="37"/>
       <c r="E17" s="41"/>
       <c r="F17" s="42"/>
       <c r="G17" s="43"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" s="38"/>
       <c r="C18" s="40"/>
     </row>
-    <row r="19" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="41"/>
       <c r="C19" s="43"/>
     </row>
@@ -4351,7 +4387,7 @@
     <mergeCell ref="B2:C3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 F5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 F5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4363,37 +4399,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="11.19921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="17"/>
       <c r="E2" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="34"/>
     </row>
-    <row r="3" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="2:8" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
@@ -4407,7 +4443,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
@@ -4415,13 +4451,13 @@
         <v>0.25</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="19" t="s">
         <v>10</v>
       </c>
@@ -4435,15 +4471,15 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="E7" s="9"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B8" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="18">
         <f>1-C4</f>
@@ -4459,7 +4495,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
@@ -4468,14 +4504,14 @@
         <v>1.9599639845400536</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="23">
         <f>1-F4</f>
         <v>0.95</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
@@ -4493,7 +4529,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B11" s="11" t="s">
         <v>0</v>
       </c>
@@ -4509,7 +4545,7 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B12" s="10" t="s">
         <v>1</v>
       </c>
@@ -4518,7 +4554,7 @@
         <v>7.6762021956290311E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B13" s="12" t="s">
         <v>2</v>
       </c>
@@ -4533,12 +4569,12 @@
       <c r="F13" s="36"/>
       <c r="G13" s="37"/>
     </row>
-    <row r="14" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E14" s="38"/>
       <c r="F14" s="39"/>
       <c r="G14" s="40"/>
     </row>
-    <row r="15" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="35" t="str">
         <f>"The mean is between "&amp;TEXT(C12,"0.00%")&amp;" and "&amp;TEXT(C13,"0.00%")&amp; " with "&amp;TEXT(C8, "0%")&amp; " confidence."</f>
         <v>The mean is between 7.68% and 42.32% with 95% confidence.</v>
@@ -4549,21 +4585,21 @@
       <c r="F15" s="39"/>
       <c r="G15" s="40"/>
     </row>
-    <row r="16" spans="2:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="38"/>
       <c r="C16" s="40"/>
       <c r="E16" s="41"/>
       <c r="F16" s="42"/>
       <c r="G16" s="43"/>
     </row>
-    <row r="17" spans="2:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="41"/>
       <c r="C17" s="43"/>
     </row>
-    <row r="19" spans="2:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="2:4" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B20" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="27" t="str">
         <f>IF(COUNTIF(C21:C22, FALSE)=0,"VALID","NOT VALID!!")</f>
@@ -4571,9 +4607,9 @@
       </c>
       <c r="D20"/>
     </row>
-    <row r="21" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B21" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="29" t="b">
         <f>IF(C5*C6 &lt; 5, FALSE,TRUE)</f>
@@ -4581,9 +4617,9 @@
       </c>
       <c r="D21"/>
     </row>
-    <row r="22" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="31" t="b">
         <f>IF((1-C5)*C6 &lt; 5, FALSE,TRUE)</f>
@@ -4598,7 +4634,7 @@
     <mergeCell ref="B15:C17"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C5 F4 F5 F6">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C5 F4 F5 F6" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4610,41 +4646,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="1" max="1" width="4.1328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1328125" style="1"/>
     <col min="4" max="4" width="5.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="5" width="23.796875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="45"/>
     </row>
-    <row r="3" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="46"/>
       <c r="C3" s="47"/>
       <c r="E3" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="33"/>
       <c r="G3" s="34"/>
     </row>
-    <row r="4" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
@@ -4658,7 +4694,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
@@ -4666,27 +4702,27 @@
         <v>12630.37</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4">
         <v>3536</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4">
         <v>5393.38</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B8" s="19" t="s">
         <v>10</v>
       </c>
@@ -4696,7 +4732,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="E9" s="9" t="s">
@@ -4708,25 +4744,25 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B10" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="18">
         <f>1-C5</f>
         <v>0.95</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="23">
         <f>1-F5</f>
         <v>0.95</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B11" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="13">
         <f>_xlfn.NORM.S.INV(1-C5/2)</f>
@@ -4741,9 +4777,9 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B12" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5">
         <f>_xlfn.CONFIDENCE.NORM(C5,C7,C8)</f>
@@ -4757,16 +4793,16 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B13" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5">
         <f>C11*C7/SQRT(C8)</f>
         <v>2157.7617514184331</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="B14" s="10" t="s">
         <v>1</v>
       </c>
@@ -4781,7 +4817,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="37"/>
     </row>
-    <row r="15" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B15" s="12" t="s">
         <v>2</v>
       </c>
@@ -4793,13 +4829,13 @@
       <c r="F15" s="39"/>
       <c r="G15" s="40"/>
     </row>
-    <row r="16" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D16" s="22"/>
       <c r="E16" s="38"/>
       <c r="F16" s="39"/>
       <c r="G16" s="40"/>
     </row>
-    <row r="17" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="35" t="str">
         <f>"The mean is between "&amp;TEXT(C14,"0.00")&amp;" and "&amp;TEXT(C15,"0.00")&amp; " with "&amp;TEXT(C10, "0%")&amp; " confidence."</f>
         <v>The mean is between 10472.61 and 14788.13 with 95% confidence.</v>
@@ -4809,15 +4845,15 @@
       <c r="F17" s="42"/>
       <c r="G17" s="43"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" s="38"/>
       <c r="C18" s="40"/>
     </row>
-    <row r="19" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="41"/>
       <c r="C19" s="43"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="str">
         <f>"The mean is between"&amp;TEXT(C14,"0.00")&amp;" and "&amp;TEXT(C15,"0.00")&amp; " with "&amp;TEXT(C10, "0%")&amp; " confidence."</f>
         <v>The mean is between10472.61 and 14788.13 with 95% confidence.</v>
@@ -4831,7 +4867,7 @@
     <mergeCell ref="B17:C19"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 F5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 F5" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>